<commit_message>
murcielago effort scratch notes
</commit_message>
<xml_diff>
--- a/data/compiling/2023/CRSR/murciélago_parcelas/Murciélago_effort_2023.xlsx
+++ b/data/compiling/2023/CRSR/murciélago_parcelas/Murciélago_effort_2023.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisjoyce/GitHub/ACG-CBC-data/data/compiling/2023/CRSR/murciélago_parcelas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C330D732-FD60-4047-93BC-4342F7C8265A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E230876-C536-214B-AC81-B286E022615A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7820" yWindow="760" windowWidth="28040" windowHeight="17140" xr2:uid="{8BA773B0-5346-2648-92B4-F339C4A77B01}"/>
+    <workbookView xWindow="2200" yWindow="760" windowWidth="28040" windowHeight="17140" xr2:uid="{8BA773B0-5346-2648-92B4-F339C4A77B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>Segment</t>
   </si>
@@ -105,6 +105,24 @@
   </si>
   <si>
     <t>16:43-17:53</t>
+  </si>
+  <si>
+    <t>total time</t>
+  </si>
+  <si>
+    <t>night time</t>
+  </si>
+  <si>
+    <t>day time</t>
+  </si>
+  <si>
+    <t>nap</t>
+  </si>
+  <si>
+    <t>walkng total</t>
+  </si>
+  <si>
+    <t>driving total</t>
   </si>
 </sst>
 </file>
@@ -466,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CE98978-A2D3-9242-9FF8-D4E22F525FE3}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -666,6 +684,77 @@
         <v>22</v>
       </c>
     </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>0.74513888888888891</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16">
+        <f>D2+D3+D7+D14</f>
+        <v>5.2200000000000006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <f>A16-A2</f>
+        <v>0.53125</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17">
+        <f>D5+D6+D10+D11+D13</f>
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>0.40625</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>